<commit_message>
Hoan thanh trang san pham va trang thanh toan, dong thoi hoan thanh api cho viec dang nhap dang ky
</commit_message>
<xml_diff>
--- a/Documents/Database Design/ExcelHelper/GenScript.xlsx
+++ b/Documents/Database Design/ExcelHelper/GenScript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectGR\Documents\Database Design\ExcelHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15ECB182-3FB3-4FDA-B80C-7B84B1CDB424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A472A4E-1C3A-4883-B834-0D5229505847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C87DE3E6-F651-417D-8998-A3CFD3A1E5EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87DE3E6-F651-417D-8998-A3CFD3A1E5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="GenScriptCategory" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
   <dimension ref="B1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B51" si="0">CONCATENATE("(",H3,",'",I3,"','",J3,"'),")</f>
+        <f t="shared" ref="B3:B52" si="0">CONCATENATE("(",H3,",'",I3,"','",J3,"'),")</f>
         <v>(UUID(),'Trái cây','7296a6c6-0fd9-11ed-8918-34415dd21b70'),</v>
       </c>
       <c r="H3" t="s">
@@ -1454,6 +1454,10 @@
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>(UUID(),'Hàng mùa vụ','861ae0b4-0fd9-11ed-8918-34415dd21b70'),</v>
+      </c>
       <c r="H52" t="s">
         <v>1</v>
       </c>
@@ -1473,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E69B67-BADA-42A8-A10A-3E2B9BF506FB}">
   <dimension ref="C1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +1943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EADA42-BFA6-4277-9965-9C89758D2337}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>

</xml_diff>